<commit_message>
Se empiezan los scrips de las tablas
Se crea un archivo txt donde van a reposar todos los scripts de creaciòn de tablespaces, datafiles, roles, usuarios y asignaciòn de permisos, tambie`n los scrips de las tablas donde se va a guadar los datos, quedo pendiente por crear los constraints de las tablas que me fueron asignadas
</commit_message>
<xml_diff>
--- a/Tablas Uber.xlsx
+++ b/Tablas Uber.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BasesDatos\Assigment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCF566C-9BF1-48DC-AF57-BCCB474317A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F86D18-A837-4AEA-81C6-0D69B464C8A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19560" windowHeight="8130" xr2:uid="{2D01F076-C3C0-4A1D-B327-24AFDFB4FF68}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8130" xr2:uid="{2D01F076-C3C0-4A1D-B327-24AFDFB4FF68}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablas" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="85">
   <si>
     <t>Id</t>
   </si>
@@ -276,6 +276,15 @@
   </si>
   <si>
     <t>Longitud</t>
+  </si>
+  <si>
+    <t>iddetallefactura</t>
+  </si>
+  <si>
+    <t>idconductor</t>
+  </si>
+  <si>
+    <t>EnviarEmail</t>
   </si>
 </sst>
 </file>
@@ -349,9 +358,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -359,6 +365,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,15 +684,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5AD93F-535F-4DCE-8B41-B949A4C1FFE2}">
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -692,22 +701,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -835,22 +844,22 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -927,6 +936,9 @@
       <c r="E18" t="s">
         <v>21</v>
       </c>
+      <c r="I18" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
@@ -953,41 +965,41 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="I25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K25" s="6" t="s">
+      <c r="K25" s="5" t="s">
         <v>54</v>
       </c>
       <c r="M25" t="s">
@@ -1013,13 +1025,13 @@
       <c r="I26" t="s">
         <v>0</v>
       </c>
-      <c r="K26" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M26" s="4" t="s">
+      <c r="K26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M26" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="O26" s="3" t="s">
+      <c r="O26" s="2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1042,10 +1054,10 @@
       <c r="K27" t="s">
         <v>55</v>
       </c>
-      <c r="M27" s="6" t="s">
+      <c r="M27" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="O27" s="8" t="s">
+      <c r="O27" s="7" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1084,7 +1096,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C30" t="s">
@@ -1106,7 +1118,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C32" t="s">
@@ -1117,7 +1129,7 @@
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C33" t="s">
@@ -1135,24 +1147,24 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1183,6 +1195,9 @@
       <c r="C41" t="s">
         <v>74</v>
       </c>
+      <c r="E41" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1234,6 +1249,9 @@
       </c>
       <c r="C46" t="s">
         <v>79</v>
+      </c>
+      <c r="E46" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>